<commit_message>
editado el archivo excel desde master
</commit_message>
<xml_diff>
--- a/ex1.xlsx
+++ b/ex1.xlsx
@@ -342,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,6 +390,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>20</v>
+      </c>
+      <c r="B6">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
editando el archivo excel desde web
</commit_message>
<xml_diff>
--- a/ex1.xlsx
+++ b/ex1.xlsx
@@ -342,10 +342,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -390,6 +390,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>